<commit_message>
re-exported all project files.
</commit_message>
<xml_diff>
--- a/Project Outputs for WordStorm Button/BOM/Bill of Materials-WordStorm Button.xlsx
+++ b/Project Outputs for WordStorm Button/BOM/Bill of Materials-WordStorm Button.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\WordStorm Button\Project Outputs for WordStorm Button\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00536195-AF8D-4106-94FB-5652C5E21ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03A885A0-62A5-4469-9A74-DC7999AD92F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="2775" windowWidth="21600" windowHeight="13065" xr2:uid="{A25B8EDE-5EFC-41FA-9DB4-B2B8ECA1C739}"/>
+    <workbookView xWindow="3615" yWindow="2775" windowWidth="21600" windowHeight="13065" xr2:uid="{C69CD0F3-DA29-4B2C-B91C-6CC7273F35EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WordStorm But" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A56FC0E-B32A-4130-9F19-F39A0EB058C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89090C5-6A26-4797-8D74-6F0F7E562DE7}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>